<commit_message>
Added Approx Category of data
</commit_message>
<xml_diff>
--- a/beginner/train_data/data_dictionary.xlsx
+++ b/beginner/train_data/data_dictionary.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\harv-matadeen\case\case_logs\Auto\Hackathon-Beginner\beginner\train_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F93FEA1-21BF-4673-881C-7ED0DBE32180}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-10965" yWindow="4200" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7midNy7LjSzABWRJlIguaeym4FDrcQ=="/>
@@ -16,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="125">
   <si>
     <t>Row_ID</t>
   </si>
@@ -370,60 +379,95 @@
   </si>
   <si>
     <t>Number of shares (target)</t>
+  </si>
+  <si>
+    <t>To Del</t>
+  </si>
+  <si>
+    <t>Numerical</t>
+  </si>
+  <si>
+    <t>Categorical</t>
+  </si>
+  <si>
+    <t>if slabs</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>Doubt</t>
+  </si>
+  <si>
+    <t>Used as per condition of Sat and Sun</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arimo"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -613,516 +657,726 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="61.11"/>
-    <col customWidth="1" min="3" max="3" width="10.56"/>
-    <col customWidth="1" min="4" max="4" width="51.33"/>
-    <col customWidth="1" min="5" max="26" width="10.56"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.109375" customWidth="1"/>
+    <col min="5" max="26" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
+      <c r="C1" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
+      <c r="C2" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
+      <c r="C3" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
+      <c r="C4" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
+      <c r="C5" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
+      <c r="C6" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
+      <c r="C7" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
+      <c r="C8" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
+      <c r="C9" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
+      <c r="C10" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
+      <c r="C11" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
+      <c r="C12" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
+      <c r="C13" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
+      <c r="C14" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
+      <c r="C15" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
+      <c r="C16" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
+      <c r="C17" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
+      <c r="C18" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
+      <c r="C19" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
+      <c r="C20" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
+      <c r="C21" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
+      <c r="C22" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
+      <c r="C23" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
+      <c r="C24" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
+      <c r="C25" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
+      <c r="C26" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
+      <c r="C27" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
+      <c r="C28" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
+      <c r="C29" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
+      <c r="C30" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
+      <c r="C31" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
+      <c r="C32" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
+      <c r="C33" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
+      <c r="C34" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
+      <c r="C35" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
+      <c r="C36" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
+      <c r="C37" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" customHeight="1">
       <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
+      <c r="C38" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
+      <c r="C39" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" customHeight="1">
       <c r="A40" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
+      <c r="C40" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" customHeight="1">
       <c r="A41" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
+      <c r="C41" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" customHeight="1">
       <c r="A42" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
+      <c r="C42" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" customHeight="1">
       <c r="A43" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
+      <c r="C43" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" customHeight="1">
       <c r="A44" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
+      <c r="C44" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" customHeight="1">
       <c r="A45" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="46" ht="15.75" customHeight="1">
+      <c r="C45" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" customHeight="1">
       <c r="A46" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="47" ht="15.75" customHeight="1">
+      <c r="C46" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" customHeight="1">
       <c r="A47" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
+      <c r="C47" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" customHeight="1">
       <c r="A48" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="49" ht="15.75" customHeight="1">
+      <c r="C48" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" customHeight="1">
       <c r="A49" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
+      <c r="C49" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" customHeight="1">
       <c r="A50" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="51" ht="15.75" customHeight="1">
+      <c r="C50" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" customHeight="1">
       <c r="A51" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="52" ht="15.75" customHeight="1">
+      <c r="C51" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" customHeight="1">
       <c r="A52" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="53" ht="15.75" customHeight="1">
+      <c r="C52" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D52" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" customHeight="1">
       <c r="A53" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
+      <c r="C53" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D53" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" customHeight="1">
       <c r="A54" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="55" ht="15.75" customHeight="1">
+      <c r="C54" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D54" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" customHeight="1">
       <c r="A55" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="56" ht="15.75" customHeight="1">
+      <c r="C55" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" customHeight="1">
       <c r="A56" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="57" ht="15.75" customHeight="1">
+      <c r="C56" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D56" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" customHeight="1">
       <c r="A57" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="58" ht="15.75" customHeight="1">
+      <c r="C57" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" customHeight="1">
       <c r="A58" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="59" ht="15.75" customHeight="1">
+      <c r="C58" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" customHeight="1">
       <c r="A59" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="60" ht="15.75" customHeight="1">
+      <c r="C59" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" customHeight="1">
       <c r="A60" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="61" ht="15.75" customHeight="1">
+      <c r="C60" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" customHeight="1">
       <c r="A61" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
+      <c r="C61" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="63" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="64" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>
     <row r="66" ht="15.75" customHeight="1"/>
     <row r="67" ht="15.75" customHeight="1"/>
@@ -2060,9 +2314,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>